<commit_message>
Working on TournamnetPairings UI
</commit_message>
<xml_diff>
--- a/Tourney Bracket Wireframe/Sample brackets.xlsx
+++ b/Tourney Bracket Wireframe/Sample brackets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbecker\Google Drive\PSU IST2\ist402(android)\team project\ist402_group\Tourney Bracket Wireframe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbecker\Google Drive\PSU IST2\ist402(android)\team project\Tourney Bracket Wireframe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -440,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,6 +477,9 @@
       <c r="L1">
         <v>0</v>
       </c>
+      <c r="M1">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -504,6 +507,9 @@
       <c r="L2">
         <v>0</v>
       </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
@@ -531,6 +537,9 @@
       <c r="L3">
         <v>0</v>
       </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -558,6 +567,9 @@
       <c r="L4" s="6">
         <v>0</v>
       </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
@@ -585,6 +597,9 @@
       <c r="L5" s="6">
         <v>0</v>
       </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -612,6 +627,9 @@
       <c r="L6" s="6">
         <v>0</v>
       </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
@@ -639,6 +657,9 @@
       <c r="L7" s="6">
         <v>0</v>
       </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -666,6 +687,9 @@
       <c r="L8" s="4">
         <v>1</v>
       </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
@@ -693,6 +717,9 @@
       <c r="L9" s="2">
         <v>0</v>
       </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -720,6 +747,9 @@
       <c r="L10" s="7">
         <v>0</v>
       </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -747,6 +777,9 @@
       <c r="L11" s="7">
         <v>0</v>
       </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -774,6 +807,9 @@
       <c r="L12" s="7">
         <v>0</v>
       </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
@@ -799,6 +835,9 @@
       <c r="L13" s="7">
         <v>0</v>
       </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -822,6 +861,9 @@
         <v>0</v>
       </c>
       <c r="L14" s="7">
+        <v>0</v>
+      </c>
+      <c r="M14">
         <v>0</v>
       </c>
     </row>
@@ -847,6 +889,9 @@
       <c r="L15" s="7">
         <v>0</v>
       </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -874,9 +919,11 @@
       <c r="L16" s="7">
         <v>0</v>
       </c>
-      <c r="M16" s="4"/>
-    </row>
-    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I17" s="1">
         <v>1</v>
       </c>
@@ -889,8 +936,11 @@
       <c r="L17" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I18" s="2">
         <v>0</v>
       </c>
@@ -904,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I19" s="3">
         <v>1</v>
       </c>
@@ -918,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I20" s="6">
         <v>0</v>
       </c>
@@ -932,7 +982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I21" s="1">
         <v>1</v>
       </c>
@@ -946,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I22" s="2">
         <v>0</v>
       </c>
@@ -960,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I23" s="3">
         <v>1</v>
       </c>
@@ -974,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I24" s="6">
         <v>0</v>
       </c>
@@ -988,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I25" s="1">
         <v>1</v>
       </c>
@@ -999,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I26" s="2">
         <v>0</v>
       </c>
@@ -1010,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I27" s="3">
         <v>1</v>
       </c>
@@ -1021,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I28" s="6">
         <v>0</v>
       </c>
@@ -1032,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I29" s="1">
         <v>1</v>
       </c>
@@ -1040,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I30" s="2">
         <v>0</v>
       </c>
@@ -1048,9 +1098,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I31" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33">
+        <v>3</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+      <c r="M33">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4 and 8 team brackets created
</commit_message>
<xml_diff>
--- a/Tourney Bracket Wireframe/Sample brackets.xlsx
+++ b/Tourney Bracket Wireframe/Sample brackets.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="4875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -21,6 +23,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>2^0 +rows</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I31" sqref="I1:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +474,9 @@
       <c r="D1" s="9">
         <v>0</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="9">
+        <v>0</v>
+      </c>
       <c r="I1" s="1">
         <v>1</v>
       </c>
@@ -494,7 +506,9 @@
       <c r="D2" s="9">
         <v>0</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
       <c r="I2" s="2">
         <v>0</v>
       </c>
@@ -524,7 +538,9 @@
       <c r="D3" s="9">
         <v>0</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
       <c r="I3" s="3">
         <v>1</v>
       </c>
@@ -554,7 +570,9 @@
       <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
       <c r="I4" s="6">
         <v>0</v>
       </c>
@@ -584,7 +602,9 @@
       <c r="D5" s="11">
         <v>0</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
       <c r="I5" s="1">
         <v>1</v>
       </c>
@@ -614,7 +634,9 @@
       <c r="D6" s="14">
         <v>0</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
       <c r="I6" s="2">
         <v>0</v>
       </c>
@@ -644,7 +666,9 @@
       <c r="D7" s="14">
         <v>0</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
       <c r="I7" s="3">
         <v>1</v>
       </c>
@@ -674,7 +698,9 @@
       <c r="D8" s="14">
         <v>0</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
       <c r="I8" s="6">
         <v>0</v>
       </c>
@@ -704,7 +730,9 @@
       <c r="D9" s="14">
         <v>0</v>
       </c>
-      <c r="E9" s="9"/>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
       <c r="I9" s="1">
         <v>1</v>
       </c>
@@ -734,7 +762,9 @@
       <c r="D10" s="14">
         <v>0</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
       <c r="I10" s="2">
         <v>0</v>
       </c>
@@ -764,7 +794,9 @@
       <c r="D11" s="14">
         <v>0</v>
       </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9">
+        <v>0</v>
+      </c>
       <c r="I11" s="3">
         <v>1</v>
       </c>
@@ -794,7 +826,9 @@
       <c r="D12" s="15">
         <v>1</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
       <c r="I12" s="6">
         <v>0</v>
       </c>
@@ -821,8 +855,12 @@
       <c r="C13" s="18">
         <v>0</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0</v>
+      </c>
       <c r="I13" s="1">
         <v>1</v>
       </c>
@@ -849,8 +887,12 @@
       <c r="C14" s="15">
         <v>1</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
       <c r="I14" s="2">
         <v>0</v>
       </c>
@@ -874,9 +916,15 @@
       <c r="B15" s="13">
         <v>1</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
       <c r="I15" s="3">
         <v>1</v>
       </c>
@@ -895,35 +943,35 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="9">
-        <v>1</v>
-      </c>
-      <c r="C16" s="9">
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="9">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9">
         <v>2</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D17" s="9">
         <v>3</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E17" s="9">
         <v>4</v>
       </c>
-      <c r="I16" s="6">
-        <v>0</v>
-      </c>
-      <c r="J16" s="6">
-        <v>0</v>
-      </c>
-      <c r="K16" s="6">
-        <v>0</v>
-      </c>
-      <c r="L16" s="7">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I17" s="1">
         <v>1</v>
       </c>
@@ -940,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I18" s="2">
         <v>0</v>
       </c>
@@ -954,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I19" s="3">
         <v>1</v>
       </c>
@@ -968,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I20" s="6">
         <v>0</v>
       </c>
@@ -982,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I21" s="1">
         <v>1</v>
       </c>
@@ -996,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I22" s="2">
         <v>0</v>
       </c>
@@ -1010,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I23" s="3">
         <v>1</v>
       </c>
@@ -1024,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I24" s="6">
         <v>0</v>
       </c>
@@ -1038,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I25" s="1">
         <v>1</v>
       </c>
@@ -1049,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I26" s="2">
         <v>0</v>
       </c>
@@ -1060,7 +1108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I27" s="3">
         <v>1</v>
       </c>
@@ -1071,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I28" s="6">
         <v>0</v>
       </c>
@@ -1082,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I29" s="1">
         <v>1</v>
       </c>
@@ -1090,7 +1138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I30" s="2">
         <v>0</v>
       </c>
@@ -1098,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I31" s="3">
         <v>1</v>
       </c>
@@ -1124,4 +1172,704 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>2^1</f>
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <f>2^2</f>
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <f>2^3</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>15</v>
+      </c>
+      <c r="J4" s="9">
+        <v>30</v>
+      </c>
+      <c r="K4" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>6</v>
+      </c>
+      <c r="D5" s="9">
+        <v>7</v>
+      </c>
+      <c r="H5" s="11">
+        <v>1</v>
+      </c>
+      <c r="I5" s="12">
+        <v>16</v>
+      </c>
+      <c r="J5" s="9">
+        <v>31</v>
+      </c>
+      <c r="K5" s="9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>8</v>
+      </c>
+      <c r="B6" s="11">
+        <v>9</v>
+      </c>
+      <c r="C6" s="9">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9">
+        <v>11</v>
+      </c>
+      <c r="H6" s="13">
+        <v>2</v>
+      </c>
+      <c r="I6" s="11">
+        <v>17</v>
+      </c>
+      <c r="J6" s="9">
+        <v>32</v>
+      </c>
+      <c r="K6" s="9">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>12</v>
+      </c>
+      <c r="B7" s="14">
+        <v>13</v>
+      </c>
+      <c r="C7" s="12">
+        <v>14</v>
+      </c>
+      <c r="D7" s="9">
+        <v>15</v>
+      </c>
+      <c r="H7" s="9">
+        <v>3</v>
+      </c>
+      <c r="I7" s="14">
+        <v>18</v>
+      </c>
+      <c r="J7" s="12">
+        <v>33</v>
+      </c>
+      <c r="K7" s="9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>16</v>
+      </c>
+      <c r="B8" s="14">
+        <v>17</v>
+      </c>
+      <c r="C8" s="11">
+        <v>18</v>
+      </c>
+      <c r="D8" s="9">
+        <v>19</v>
+      </c>
+      <c r="H8" s="10">
+        <v>4</v>
+      </c>
+      <c r="I8" s="14">
+        <v>19</v>
+      </c>
+      <c r="J8" s="11">
+        <v>34</v>
+      </c>
+      <c r="K8" s="9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>20</v>
+      </c>
+      <c r="B9" s="15">
+        <v>21</v>
+      </c>
+      <c r="C9" s="14">
+        <v>22</v>
+      </c>
+      <c r="D9" s="9">
+        <v>23</v>
+      </c>
+      <c r="H9" s="11">
+        <v>5</v>
+      </c>
+      <c r="I9" s="15">
+        <v>20</v>
+      </c>
+      <c r="J9" s="14">
+        <v>35</v>
+      </c>
+      <c r="K9" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>24</v>
+      </c>
+      <c r="B10" s="16">
+        <v>25</v>
+      </c>
+      <c r="C10" s="14">
+        <v>26</v>
+      </c>
+      <c r="D10" s="9">
+        <v>27</v>
+      </c>
+      <c r="H10" s="13">
+        <v>6</v>
+      </c>
+      <c r="I10" s="16">
+        <v>21</v>
+      </c>
+      <c r="J10" s="14">
+        <v>36</v>
+      </c>
+      <c r="K10" s="9">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>28</v>
+      </c>
+      <c r="B11" s="16">
+        <v>29</v>
+      </c>
+      <c r="C11" s="14">
+        <v>30</v>
+      </c>
+      <c r="D11" s="12">
+        <v>31</v>
+      </c>
+      <c r="H11" s="9">
+        <v>7</v>
+      </c>
+      <c r="I11" s="16">
+        <v>22</v>
+      </c>
+      <c r="J11" s="14">
+        <v>37</v>
+      </c>
+      <c r="K11" s="12">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>32</v>
+      </c>
+      <c r="B12" s="16">
+        <v>33</v>
+      </c>
+      <c r="C12" s="14">
+        <v>34</v>
+      </c>
+      <c r="D12" s="9">
+        <v>35</v>
+      </c>
+      <c r="H12" s="10">
+        <v>8</v>
+      </c>
+      <c r="I12" s="16">
+        <v>23</v>
+      </c>
+      <c r="J12" s="14">
+        <v>38</v>
+      </c>
+      <c r="K12" s="9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>36</v>
+      </c>
+      <c r="B13" s="12">
+        <v>37</v>
+      </c>
+      <c r="C13" s="14">
+        <v>38</v>
+      </c>
+      <c r="D13" s="9">
+        <v>39</v>
+      </c>
+      <c r="H13" s="11">
+        <v>9</v>
+      </c>
+      <c r="I13" s="12">
+        <v>24</v>
+      </c>
+      <c r="J13" s="14">
+        <v>39</v>
+      </c>
+      <c r="K13" s="9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>40</v>
+      </c>
+      <c r="B14" s="17">
+        <v>41</v>
+      </c>
+      <c r="C14" s="14">
+        <v>42</v>
+      </c>
+      <c r="D14" s="9">
+        <v>43</v>
+      </c>
+      <c r="H14" s="13">
+        <v>10</v>
+      </c>
+      <c r="I14" s="17">
+        <v>25</v>
+      </c>
+      <c r="J14" s="14">
+        <v>40</v>
+      </c>
+      <c r="K14" s="9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>44</v>
+      </c>
+      <c r="B15" s="18">
+        <v>45</v>
+      </c>
+      <c r="C15" s="15">
+        <v>46</v>
+      </c>
+      <c r="D15" s="9">
+        <v>47</v>
+      </c>
+      <c r="H15" s="9">
+        <v>11</v>
+      </c>
+      <c r="I15" s="18">
+        <v>26</v>
+      </c>
+      <c r="J15" s="15">
+        <v>41</v>
+      </c>
+      <c r="K15" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>48</v>
+      </c>
+      <c r="B16" s="18">
+        <v>49</v>
+      </c>
+      <c r="C16" s="9">
+        <v>50</v>
+      </c>
+      <c r="D16" s="9">
+        <v>51</v>
+      </c>
+      <c r="H16" s="10">
+        <v>12</v>
+      </c>
+      <c r="I16" s="18">
+        <v>27</v>
+      </c>
+      <c r="J16" s="9">
+        <v>42</v>
+      </c>
+      <c r="K16" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>52</v>
+      </c>
+      <c r="B17" s="15">
+        <v>53</v>
+      </c>
+      <c r="C17" s="9">
+        <v>54</v>
+      </c>
+      <c r="D17" s="9">
+        <v>55</v>
+      </c>
+      <c r="H17" s="11">
+        <v>13</v>
+      </c>
+      <c r="I17" s="15">
+        <v>28</v>
+      </c>
+      <c r="J17" s="9">
+        <v>43</v>
+      </c>
+      <c r="K17" s="9">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>56</v>
+      </c>
+      <c r="B18" s="9">
+        <v>57</v>
+      </c>
+      <c r="C18" s="9">
+        <v>58</v>
+      </c>
+      <c r="D18" s="9">
+        <v>59</v>
+      </c>
+      <c r="H18" s="13">
+        <v>14</v>
+      </c>
+      <c r="I18" s="9">
+        <v>29</v>
+      </c>
+      <c r="J18" s="9">
+        <v>44</v>
+      </c>
+      <c r="K18" s="9">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>16</v>
+      </c>
+      <c r="B4" s="7">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6">
+        <v>19</v>
+      </c>
+      <c r="E4" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>21</v>
+      </c>
+      <c r="B5" s="7">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>26</v>
+      </c>
+      <c r="B6" s="8">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7">
+        <v>28</v>
+      </c>
+      <c r="D6" s="6">
+        <v>29</v>
+      </c>
+      <c r="E6" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6">
+        <v>32</v>
+      </c>
+      <c r="C7" s="7">
+        <v>33</v>
+      </c>
+      <c r="D7" s="6">
+        <v>34</v>
+      </c>
+      <c r="E7" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>36</v>
+      </c>
+      <c r="B8" s="6">
+        <v>37</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>